<commit_message>
onprogress save to excel
</commit_message>
<xml_diff>
--- a/backend/Simple.xlsx
+++ b/backend/Simple.xlsx
@@ -2,40 +2,33 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
+  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -48,13 +41,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
@@ -318,31 +311,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>No</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Nama</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Alasan</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Start</v>
-      </c>
-      <c r="E1" t="str">
-        <v>End</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetData/>
 </worksheet>
 </file>
</xml_diff>